<commit_message>
finalised constructing data with aggregating
</commit_message>
<xml_diff>
--- a/DownloadDataForDK/ModelData/E2H.xlsx
+++ b/DownloadDataForDK/ModelData/E2H.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,27 +448,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Biogas</t>
+          <t>id_DK_Central_BP_Biogas</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8958690272225396</v>
+        <v>0.9040708221464335</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Biomass</t>
+          <t>id_DK_Central_BP_Biomass</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5042074830085307</v>
+        <v>0.5191079496755285</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Coal</t>
+          <t>id_DK_Central_BP_Coal</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,37 +478,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Natgas</t>
+          <t>id_DK_Central_BP_Natgas</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8509450978383946</v>
+        <v>0.8853056785872065</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Oil</t>
+          <t>id_DK_Central_BP_Oil</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.029915912031048</v>
+        <v>0.929567474048443</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>id_DK1_Central_BP_Waste</t>
+          <t>id_DK_Central_BP_Waste</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2023212054348749</v>
+        <v>0.2170321674969613</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>id_DK1_Central_EP</t>
+          <t>id_DK_Central_EP</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -518,27 +518,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>id_DK1_Central_HPstandard</t>
+          <t>id_DK_Central_HPstandard</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.2808402594568861</v>
+        <v>-0.2835696120719935</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>id_DK1_Central_HPsurplusheat</t>
+          <t>id_DK_Central_HPsurplusheat</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.2471153414447986</v>
+        <v>-0.2264675350768509</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>id_DK1_Central_IH</t>
+          <t>id_DK_Central_IH</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,57 +548,57 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_BP_Biogas</t>
+          <t>id_DK_Decentral_BP_Biogas</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5846440949080245</v>
+        <v>0.8183245501460831</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_BP_Biomass</t>
+          <t>id_DK_Decentral_BP_Biomass</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.286123618501842</v>
+        <v>0.2502852161001509</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_BP_Natgas</t>
+          <t>id_DK_Decentral_BP_Natgas</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9722387812787902</v>
+        <v>0.8341355209302362</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_BP_Oil</t>
+          <t>id_DK_Decentral_BP_Oil</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.08855585831062671</v>
+        <v>0.9680836676734437</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_BP_Waste</t>
+          <t>id_DK_Decentral_BP_Waste</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.169056424658347</v>
+        <v>0.2009654150636156</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_EP</t>
+          <t>id_DK_Decentral_EP</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -608,330 +608,30 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_HPstandard</t>
+          <t>id_DK_Decentral_HPstandard</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.3113682161510096</v>
+        <v>-0.2988356135312177</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_HPsurplusheat</t>
+          <t>id_DK_Decentral_HPsurplusheat</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.1848692749860931</v>
+        <v>-0.1945622349713146</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>id_DK1_LargeDecentral_IH</t>
+          <t>id_DK_Decentral_IH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_BP_Biogas</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.8505353955978585</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_BP_Biomass</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.184708050694484</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_BP_Natgas</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.7580668368565406</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_BP_Oil</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>1.068244635408815</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_BP_Waste</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>0.106756904268093</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_EP</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_HPstandard</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>-0.2929720248650695</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_HPsurplusheat</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>-0.2080392391434382</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>id_DK1_SmallDecentral_IH</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_BP_Biogas</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>0.930381679389313</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_BP_Biomass</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0.5307487094000287</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_BP_Natgas</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1.019655828336874</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_BP_Oil</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>0.3334534101825168</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_BP_Waste</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>0.2310257573690906</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_HPstandard</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>-0.2901974951830443</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_HPsurplusheat</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>-0.1658761528326746</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>id_DK2_Central_IH</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_BP_Biomass</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>0.2321046160360228</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_BP_Natgas</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>0.896144897121219</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_BP_Oil</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>0.2258064516129032</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_BP_Waste</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>0.2907210677396403</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_HPstandard</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>-0.29412</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_HPsurplusheat</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>-0.1855555555555556</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>id_DK2_LargeDecentral_IH</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_BP_Biogas</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>0.892931323283082</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_BP_Biomass</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>0.3062970186681527</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_BP_Natgas</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>0.8030666898393187</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_BP_Oil</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_HPstandard</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>-0.309554234769688</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>id_DK2_SmallDecentral_IH</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished aggregating g_H and building counterfactuals
</commit_message>
<xml_diff>
--- a/DownloadDataForDK/ModelData/E2H.xlsx
+++ b/DownloadDataForDK/ModelData/E2H.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9040708221464335</v>
+        <v>0.8319027428269387</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.5191079496755285</v>
+        <v>0.4953909906185326</v>
       </c>
     </row>
     <row r="4">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8853056785872065</v>
+        <v>0.8552075670435977</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.929567474048443</v>
+        <v>0.9402498030831551</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2170321674969613</v>
+        <v>0.2122967701559634</v>
       </c>
     </row>
     <row r="8">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.2835696120719935</v>
+        <v>-0.2949992232077283</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.2264675350768509</v>
+        <v>-0.2184503140238934</v>
       </c>
     </row>
     <row r="11">
@@ -542,96 +542,6 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_BP_Biogas</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.8183245501460831</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_BP_Biomass</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.2502852161001509</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_BP_Natgas</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.8341355209302362</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_BP_Oil</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.9680836676734437</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_BP_Waste</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.2009654150636156</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_EP</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_HPstandard</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>-0.2988356135312177</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_HPsurplusheat</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>-0.1945622349713146</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>id_DK_Decentral_IH</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
         <v>-1</v>
       </c>
     </row>

</xml_diff>